<commit_message>
Update Code for loading and plotting 20mm
</commit_message>
<xml_diff>
--- a/DataCollection/BPArecordings.xlsx
+++ b/DataCollection/BPArecordings.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawre\Documents\GitHub\Muscle-Sensory\DataCollection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D24438E-0D10-47F1-AD81-53EAFBDBCE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36253DED-7C57-4D81-8661-78CD4367D072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11760" yWindow="-11280" windowWidth="17280" windowHeight="9384" xr2:uid="{9DEA6101-A446-4647-B876-48EF8758AC2E}"/>
+    <workbookView xWindow="-41970" yWindow="4530" windowWidth="21600" windowHeight="11385" xr2:uid="{9DEA6101-A446-4647-B876-48EF8758AC2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Optimiaztion Parameters" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>BPA Diameter</t>
   </si>
@@ -143,6 +142,30 @@
   </si>
   <si>
     <t>69mm</t>
+  </si>
+  <si>
+    <t>10mm13cmUnkink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Fit (y=mx+c) </t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>10mm13cm4mm</t>
+  </si>
+  <si>
+    <t>10mm13cm8mm</t>
+  </si>
+  <si>
+    <t>10mm13cm12mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try poreto search </t>
   </si>
 </sst>
 </file>
@@ -334,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -351,6 +374,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,15 +695,15 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -687,7 +714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -707,7 +734,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="12" t="s">
         <v>5</v>
@@ -723,7 +750,7 @@
       </c>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="12" t="s">
         <v>6</v>
@@ -741,7 +768,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="11" t="s">
         <v>7</v>
@@ -759,7 +786,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="11" t="s">
         <v>8</v>
@@ -777,7 +804,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -795,7 +822,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="10" t="s">
         <v>11</v>
@@ -811,7 +838,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="10" t="s">
         <v>5</v>
@@ -827,7 +854,7 @@
       </c>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="10" t="s">
         <v>8</v>
@@ -845,7 +872,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="11" t="s">
         <v>12</v>
@@ -862,6 +889,135 @@
       <c r="F11" s="8" t="s">
         <v>35</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3326FA8-84A5-4919-8DDB-96A6DA3836F2}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="C2" s="3">
+        <v>-58.642299999999999</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.64070000000000005</v>
+      </c>
+      <c r="C3" s="5">
+        <v>-125.3122</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.58689999999999998</v>
+      </c>
+      <c r="C4" s="5">
+        <v>-191.45930000000001</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.54510000000000003</v>
+      </c>
+      <c r="C5" s="19">
+        <v>-236.8689</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Optimizing and fixing 20mm data
</commit_message>
<xml_diff>
--- a/DataCollection/BPArecordings.xlsx
+++ b/DataCollection/BPArecordings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36253DED-7C57-4D81-8661-78CD4367D072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2549DA5-C08E-41AA-9465-97A17DEEAB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41970" yWindow="4530" windowWidth="21600" windowHeight="11385" xr2:uid="{9DEA6101-A446-4647-B876-48EF8758AC2E}"/>
+    <workbookView xWindow="-26625" yWindow="2025" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{9DEA6101-A446-4647-B876-48EF8758AC2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
   <si>
     <t>BPA Diameter</t>
   </si>
@@ -166,6 +166,102 @@
   </si>
   <si>
     <t xml:space="preserve">try poreto search </t>
+  </si>
+  <si>
+    <t>10mm23cmUnkink</t>
+  </si>
+  <si>
+    <t>10mm23cm14mm</t>
+  </si>
+  <si>
+    <t>10mm23cm30mm</t>
+  </si>
+  <si>
+    <t>10mm27cmUnkink</t>
+  </si>
+  <si>
+    <t>10mm27cm7mm</t>
+  </si>
+  <si>
+    <t>10mm27cm15mm</t>
+  </si>
+  <si>
+    <t>10mm27cm31mm</t>
+  </si>
+  <si>
+    <t>10mm29cmUnkink</t>
+  </si>
+  <si>
+    <t>10mm29cm17mm</t>
+  </si>
+  <si>
+    <t>10mm29cm28mm</t>
+  </si>
+  <si>
+    <t>10mm29cm41mm</t>
+  </si>
+  <si>
+    <t>10mm30cmUnkink</t>
+  </si>
+  <si>
+    <t>10mm30cm12mm</t>
+  </si>
+  <si>
+    <t>10mm30cm22mm</t>
+  </si>
+  <si>
+    <t>10mm30cm33mm</t>
+  </si>
+  <si>
+    <t>20mm10cmUnkink</t>
+  </si>
+  <si>
+    <t>20mm10cm13mm</t>
+  </si>
+  <si>
+    <t>20mm10cm20mm</t>
+  </si>
+  <si>
+    <t>20mm12cmUnkink</t>
+  </si>
+  <si>
+    <t>20mm12cm10mm</t>
+  </si>
+  <si>
+    <t>20mm12cm20mm</t>
+  </si>
+  <si>
+    <t>20mm23cmUnkink</t>
+  </si>
+  <si>
+    <t>20mm23cm9mm</t>
+  </si>
+  <si>
+    <t>20mm23cm19mm</t>
+  </si>
+  <si>
+    <t>20mm30cmUnkink</t>
+  </si>
+  <si>
+    <t>20mm30cm14mm</t>
+  </si>
+  <si>
+    <t>20mm30cm23mm</t>
+  </si>
+  <si>
+    <t>20mm30cm34mm</t>
+  </si>
+  <si>
+    <t>20mm40cmUnkink</t>
+  </si>
+  <si>
+    <t>20mm40cm35mm</t>
+  </si>
+  <si>
+    <t>20mm40cm46mm</t>
+  </si>
+  <si>
+    <t>20mm40cm69mm</t>
   </si>
 </sst>
 </file>
@@ -357,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -378,6 +474,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,6 +491,1173 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Comparing Gradient</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-5B2E-4D03-ADFE-D472C8F92C91}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-5B2E-4D03-ADFE-D472C8F92C91}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-5B2E-4D03-ADFE-D472C8F92C91}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-5B2E-4D03-ADFE-D472C8F92C91}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-5B2E-4D03-ADFE-D472C8F92C91}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-5B2E-4D03-ADFE-D472C8F92C91}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-5B2E-4D03-ADFE-D472C8F92C91}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'Optimiaztion Parameters'!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10mm13cmUnkink</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10mm13cm4mm</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10mm13cm8mm</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10mm13cm12mm</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10mm23cmUnkink</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10mm23cm14mm</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10mm23cm30mm</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10mm27cmUnkink</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10mm27cm7mm</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10mm27cm15mm</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10mm27cm31mm</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10mm29cmUnkink</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10mm29cm17mm</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10mm29cm28mm</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10mm29cm41mm</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10mm30cmUnkink</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10mm30cm12mm</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10mm30cm22mm</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10mm30cm33mm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Optimiaztion Parameters'!$B$2:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.64700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.64070000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.58689999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54510000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.69210000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66959999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69689999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.67090000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7167</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.68799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.63470000000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.69950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.70609999999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.63360000000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.70650000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.72819999999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.68410000000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.6341</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B2E-4D03-ADFE-D472C8F92C91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="445727064"/>
+        <c:axId val="445731328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="445727064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="445731328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="445731328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="445727064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>200024</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B6AB0E4-4C58-0C93-1AAE-833EC592D903}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -694,8 +1959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47969D8-EAD2-4450-AED1-4AC2B2C485A9}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,10 +2162,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3326FA8-84A5-4919-8DDB-96A6DA3836F2}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,46 +2245,318 @@
       <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
+      <c r="A6" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.69210000000000005</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-54.6111</v>
+      </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="15"/>
+      <c r="A7" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.66959999999999997</v>
+      </c>
+      <c r="C7" s="21">
+        <v>-261.48649999999998</v>
+      </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="15"/>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.69689999999999996</v>
+      </c>
+      <c r="C8" s="19">
+        <v>-399.2253</v>
+      </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="15"/>
+      <c r="A9" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.67090000000000005</v>
+      </c>
+      <c r="C9" s="21">
+        <v>-32.126600000000003</v>
+      </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
+      <c r="A10" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.7167</v>
+      </c>
+      <c r="C10" s="5">
+        <v>-186.11670000000001</v>
+      </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="C11" s="5">
+        <v>-240.66399999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.63470000000000004</v>
+      </c>
+      <c r="C12" s="8">
+        <v>-332.35489999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.69950000000000001</v>
+      </c>
+      <c r="C13" s="3">
+        <v>-14.598800000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.70609999999999995</v>
+      </c>
+      <c r="C14" s="5">
+        <v>-218.50139999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.61</v>
+      </c>
+      <c r="C15" s="5">
+        <v>-265.43579999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.63360000000000005</v>
+      </c>
+      <c r="C16" s="8">
+        <v>-361.0643</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.70650000000000002</v>
+      </c>
+      <c r="C17" s="5">
+        <v>-31.057600000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0.72819999999999996</v>
+      </c>
+      <c r="C18" s="5">
+        <v>-230.85159999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.68410000000000004</v>
+      </c>
+      <c r="C19" s="5">
+        <v>-280.02960000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.6341</v>
+      </c>
+      <c r="C20" s="8">
+        <v>-321.22550000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.7096</v>
+      </c>
+      <c r="C21" s="3">
+        <v>-116.4791</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="C22" s="5">
+        <v>-245.39590000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="C23" s="8">
+        <v>-258.06020000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Assigning States for Pressurizing and Depressurizing
</commit_message>
<xml_diff>
--- a/DataCollection/BPArecordings.xlsx
+++ b/DataCollection/BPArecordings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7E5ADB-A7F3-4269-A547-89630CEAB106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1B3145-30CD-4386-B851-981455784E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DEA6101-A446-4647-B876-48EF8758AC2E}"/>
+    <workbookView xWindow="-10590" yWindow="2760" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="2" xr2:uid="{9DEA6101-A446-4647-B876-48EF8758AC2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="89">
   <si>
     <t>BPA Diameter</t>
   </si>
@@ -281,6 +281,27 @@
   </si>
   <si>
     <t>Force = m*pressure + c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Fit </t>
+  </si>
+  <si>
+    <t>a0</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>SSE</t>
+  </si>
+  <si>
+    <t>Model = (a0 +a1*(li-lo)/lo)*Pressure + a2*(li-lo)/lo +a3</t>
+  </si>
+  <si>
+    <t>a3</t>
   </si>
 </sst>
 </file>
@@ -296,7 +317,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,6 +333,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -533,6 +560,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5059,8 +5091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47969D8-EAD2-4450-AED1-4AC2B2C485A9}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5454,7 +5486,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5910,14 +5942,125 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13465C1-23EC-4857-B656-D16475C8BE6C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="36"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.64695999999999998</v>
+      </c>
+      <c r="C3" s="2">
+        <v>604.85</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-12.321999999999999</v>
+      </c>
+      <c r="E3" s="15">
+        <v>-58.642000000000003</v>
+      </c>
+      <c r="F3" s="39">
+        <v>110610</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4">
+        <v>-1537.6</v>
+      </c>
+      <c r="C4" s="16">
+        <v>-46146</v>
+      </c>
+      <c r="D4" s="5">
+        <v>-1106.2</v>
+      </c>
+      <c r="E4" s="39">
+        <v>-162.19</v>
+      </c>
+      <c r="F4">
+        <v>99683</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="4">
+        <v>82.831000000000003</v>
+      </c>
+      <c r="C5" s="16">
+        <v>1233.7</v>
+      </c>
+      <c r="D5" s="5">
+        <v>206.34</v>
+      </c>
+      <c r="E5" s="39">
+        <v>-177.7</v>
+      </c>
+      <c r="F5" s="39">
+        <v>110100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="18">
+        <v>49.866999999999997</v>
+      </c>
+      <c r="C6" s="38">
+        <v>493.21</v>
+      </c>
+      <c r="D6" s="8">
+        <v>122.6</v>
+      </c>
+      <c r="E6" s="39">
+        <v>-224.61</v>
+      </c>
+      <c r="F6" s="15">
+        <v>92490</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>